<commit_message>
adding high voltage and current tests
</commit_message>
<xml_diff>
--- a/data/DobleF6150.xlsx
+++ b/data/DobleF6150.xlsx
@@ -462,7 +462,7 @@
         <v>25.075</v>
       </c>
       <c r="E2" t="n">
-        <v>24.99836349</v>
+        <v>24.9979763</v>
       </c>
       <c r="F2">
         <f>IF(AND(E2&gt;=C2,E2&lt;=D2), "PASS", "FAIL")</f>
@@ -480,7 +480,7 @@
         <v>50.15</v>
       </c>
       <c r="E3" t="n">
-        <v>49.99892044</v>
+        <v>49.99749374</v>
       </c>
       <c r="F3">
         <f>IF(AND(E3&gt;=C3,E3&lt;=D3), "PASS", "FAIL")</f>
@@ -498,7 +498,7 @@
         <v>75.22499999999999</v>
       </c>
       <c r="E4" t="n">
-        <v>74.99632262999999</v>
+        <v>74.99463654</v>
       </c>
       <c r="F4">
         <f>IF(AND(E4&gt;=C4,E4&lt;=D4), "PASS", "FAIL")</f>
@@ -516,7 +516,7 @@
         <v>100.3</v>
       </c>
       <c r="E5" t="n">
-        <v>99.9958725</v>
+        <v>99.99442291</v>
       </c>
       <c r="F5">
         <f>IF(AND(E5&gt;=C5,E5&lt;=D5), "PASS", "FAIL")</f>
@@ -534,7 +534,7 @@
         <v>125.375</v>
       </c>
       <c r="E6" t="n">
-        <v>124.99278259</v>
+        <v>124.99074554</v>
       </c>
       <c r="F6">
         <f>IF(AND(E6&gt;=C6,E6&lt;=D6), "PASS", "FAIL")</f>
@@ -552,7 +552,7 @@
         <v>150.45</v>
       </c>
       <c r="E7" t="n">
-        <v>149.98980713</v>
+        <v>149.98817444</v>
       </c>
       <c r="F7">
         <f>IF(AND(E7&gt;=C7,E7&lt;=D7), "PASS", "FAIL")</f>
@@ -575,7 +575,7 @@
         <v>25.075</v>
       </c>
       <c r="E8" t="n">
-        <v>25.01109695</v>
+        <v>25.01117325</v>
       </c>
       <c r="F8">
         <f>IF(AND(E8&gt;=C8,E8&lt;=D8), "PASS", "FAIL")</f>
@@ -593,7 +593,7 @@
         <v>50.15</v>
       </c>
       <c r="E9" t="n">
-        <v>50.02330017</v>
+        <v>50.02285767</v>
       </c>
       <c r="F9">
         <f>IF(AND(E9&gt;=C9,E9&lt;=D9), "PASS", "FAIL")</f>
@@ -611,7 +611,7 @@
         <v>75.22499999999999</v>
       </c>
       <c r="E10" t="n">
-        <v>75.03429413000001</v>
+        <v>75.03379821999999</v>
       </c>
       <c r="F10">
         <f>IF(AND(E10&gt;=C10,E10&lt;=D10), "PASS", "FAIL")</f>
@@ -629,7 +629,7 @@
         <v>100.3</v>
       </c>
       <c r="E11" t="n">
-        <v>100.0484314</v>
+        <v>100.04698944</v>
       </c>
       <c r="F11">
         <f>IF(AND(E11&gt;=C11,E11&lt;=D11), "PASS", "FAIL")</f>
@@ -647,7 +647,7 @@
         <v>125.375</v>
       </c>
       <c r="E12" t="n">
-        <v>125.06186676</v>
+        <v>125.06109619</v>
       </c>
       <c r="F12">
         <f>IF(AND(E12&gt;=C12,E12&lt;=D12), "PASS", "FAIL")</f>
@@ -665,7 +665,7 @@
         <v>150.45</v>
       </c>
       <c r="E13" t="n">
-        <v>150.07234192</v>
+        <v>150.07202148</v>
       </c>
       <c r="F13">
         <f>IF(AND(E13&gt;=C13,E13&lt;=D13), "PASS", "FAIL")</f>
@@ -688,7 +688,7 @@
         <v>25.075</v>
       </c>
       <c r="E14" t="n">
-        <v>24.99135017</v>
+        <v>24.99144936</v>
       </c>
       <c r="F14">
         <f>IF(AND(E14&gt;=C14,E14&lt;=D14), "PASS", "FAIL")</f>
@@ -706,7 +706,7 @@
         <v>50.15</v>
       </c>
       <c r="E15" t="n">
-        <v>49.98639679</v>
+        <v>49.98563385</v>
       </c>
       <c r="F15">
         <f>IF(AND(E15&gt;=C15,E15&lt;=D15), "PASS", "FAIL")</f>
@@ -724,7 +724,7 @@
         <v>75.22499999999999</v>
       </c>
       <c r="E16" t="n">
-        <v>74.97821808</v>
+        <v>74.97724915000001</v>
       </c>
       <c r="F16">
         <f>IF(AND(E16&gt;=C16,E16&lt;=D16), "PASS", "FAIL")</f>
@@ -742,7 +742,7 @@
         <v>100.3</v>
       </c>
       <c r="E17" t="n">
-        <v>99.97256470000001</v>
+        <v>99.97194672000001</v>
       </c>
       <c r="F17">
         <f>IF(AND(E17&gt;=C17,E17&lt;=D17), "PASS", "FAIL")</f>
@@ -760,7 +760,7 @@
         <v>125.375</v>
       </c>
       <c r="E18" t="n">
-        <v>124.9666748</v>
+        <v>124.96549988</v>
       </c>
       <c r="F18">
         <f>IF(AND(E18&gt;=C18,E18&lt;=D18), "PASS", "FAIL")</f>
@@ -778,7 +778,7 @@
         <v>150.45</v>
       </c>
       <c r="E19" t="n">
-        <v>149.95716858</v>
+        <v>149.95675659</v>
       </c>
       <c r="F19">
         <f>IF(AND(E19&gt;=C19,E19&lt;=D19), "PASS", "FAIL")</f>
@@ -914,7 +914,7 @@
         <v>25.075</v>
       </c>
       <c r="E26" t="n">
-        <v>25.01117325</v>
+        <v>25.00974274</v>
       </c>
       <c r="F26">
         <f>IF(AND(E26&gt;=C26,E26&lt;=D26), "PASS", "FAIL")</f>
@@ -932,7 +932,7 @@
         <v>50.15</v>
       </c>
       <c r="E27" t="n">
-        <v>50.02285767</v>
+        <v>50.01837158</v>
       </c>
       <c r="F27">
         <f>IF(AND(E27&gt;=C27,E27&lt;=D27), "PASS", "FAIL")</f>
@@ -950,7 +950,7 @@
         <v>75.22499999999999</v>
       </c>
       <c r="E28" t="n">
-        <v>75.03379821999999</v>
+        <v>75.02858734</v>
       </c>
       <c r="F28">
         <f>IF(AND(E28&gt;=C28,E28&lt;=D28), "PASS", "FAIL")</f>
@@ -968,7 +968,7 @@
         <v>100.3</v>
       </c>
       <c r="E29" t="n">
-        <v>100.04698944</v>
+        <v>100.03844452</v>
       </c>
       <c r="F29">
         <f>IF(AND(E29&gt;=C29,E29&lt;=D29), "PASS", "FAIL")</f>
@@ -986,7 +986,7 @@
         <v>125.375</v>
       </c>
       <c r="E30" t="n">
-        <v>125.06109619</v>
+        <v>125.05028534</v>
       </c>
       <c r="F30">
         <f>IF(AND(E30&gt;=C30,E30&lt;=D30), "PASS", "FAIL")</f>
@@ -1004,7 +1004,7 @@
         <v>150.45</v>
       </c>
       <c r="E31" t="n">
-        <v>150.07202148</v>
+        <v>150.06365967</v>
       </c>
       <c r="F31">
         <f>IF(AND(E31&gt;=C31,E31&lt;=D31), "PASS", "FAIL")</f>
@@ -1027,7 +1027,7 @@
         <v>25.075</v>
       </c>
       <c r="E32" t="n">
-        <v>24.99144936</v>
+        <v>25.00335503</v>
       </c>
       <c r="F32">
         <f>IF(AND(E32&gt;=C32,E32&lt;=D32), "PASS", "FAIL")</f>
@@ -1045,7 +1045,7 @@
         <v>50.15</v>
       </c>
       <c r="E33" t="n">
-        <v>49.98563385</v>
+        <v>50.00356293</v>
       </c>
       <c r="F33">
         <f>IF(AND(E33&gt;=C33,E33&lt;=D33), "PASS", "FAIL")</f>
@@ -1063,7 +1063,7 @@
         <v>75.22499999999999</v>
       </c>
       <c r="E34" t="n">
-        <v>74.97724915000001</v>
+        <v>75.00463867000001</v>
       </c>
       <c r="F34">
         <f>IF(AND(E34&gt;=C34,E34&lt;=D34), "PASS", "FAIL")</f>
@@ -1081,7 +1081,7 @@
         <v>100.3</v>
       </c>
       <c r="E35" t="n">
-        <v>99.97194672000001</v>
+        <v>100.01135254</v>
       </c>
       <c r="F35">
         <f>IF(AND(E35&gt;=C35,E35&lt;=D35), "PASS", "FAIL")</f>
@@ -1099,7 +1099,7 @@
         <v>125.375</v>
       </c>
       <c r="E36" t="n">
-        <v>124.96549988</v>
+        <v>125.01959991</v>
       </c>
       <c r="F36">
         <f>IF(AND(E36&gt;=C36,E36&lt;=D36), "PASS", "FAIL")</f>
@@ -1117,7 +1117,7 @@
         <v>150.45</v>
       </c>
       <c r="E37" t="n">
-        <v>149.95675659</v>
+        <v>150.02742004</v>
       </c>
       <c r="F37">
         <f>IF(AND(E37&gt;=C37,E37&lt;=D37), "PASS", "FAIL")</f>
@@ -1818,7 +1818,7 @@
         <v>60.25</v>
       </c>
       <c r="E74" t="n">
-        <v>60.22749975459408</v>
+        <v>60.26304637721221</v>
       </c>
       <c r="F74">
         <f>IF(AND(E74&gt;=C74,E74&lt;=D74), "PASS", "FAIL")</f>
@@ -1836,7 +1836,7 @@
         <v>120.25</v>
       </c>
       <c r="E75" t="n">
-        <v>119.71249916623</v>
+        <v>120.2972119614733</v>
       </c>
       <c r="F75">
         <f>IF(AND(E75&gt;=C75,E75&lt;=D75), "PASS", "FAIL")</f>
@@ -1854,7 +1854,7 @@
         <v>180.25</v>
       </c>
       <c r="E76" t="n">
-        <v>179.768394454297</v>
+        <v>179.7593575491723</v>
       </c>
       <c r="F76">
         <f>IF(AND(E76&gt;=C76,E76&lt;=D76), "PASS", "FAIL")</f>
@@ -1877,7 +1877,7 @@
         <v>60.25</v>
       </c>
       <c r="E77" t="n">
-        <v>60.2064123855618</v>
+        <v>60.23295852263566</v>
       </c>
       <c r="F77">
         <f>IF(AND(E77&gt;=C77,E77&lt;=D77), "PASS", "FAIL")</f>
@@ -1895,7 +1895,7 @@
         <v>120.25</v>
       </c>
       <c r="E78" t="n">
-        <v>119.7535582088264</v>
+        <v>120.2331134184667</v>
       </c>
       <c r="F78">
         <f>IF(AND(E78&gt;=C78,E78&lt;=D78), "PASS", "FAIL")</f>
@@ -1913,7 +1913,7 @@
         <v>180.25</v>
       </c>
       <c r="E79" t="n">
-        <v>179.8466868971983</v>
+        <v>179.768394454297</v>
       </c>
       <c r="F79">
         <f>IF(AND(E79&gt;=C79,E79&lt;=D79), "PASS", "FAIL")</f>
@@ -1936,7 +1936,7 @@
         <v>60.25</v>
       </c>
       <c r="E80" t="n">
-        <v>59.81946758261149</v>
+        <v>60.21943581112865</v>
       </c>
       <c r="F80">
         <f>IF(AND(E80&gt;=C80,E80&lt;=D80), "PASS", "FAIL")</f>
@@ -1954,7 +1954,7 @@
         <v>120.25</v>
       </c>
       <c r="E81" t="n">
-        <v>119.7796083109589</v>
+        <v>120.2084549933066</v>
       </c>
       <c r="F81">
         <f>IF(AND(E81&gt;=C81,E81&lt;=D81), "PASS", "FAIL")</f>
@@ -1972,7 +1972,7 @@
         <v>180.25</v>
       </c>
       <c r="E82" t="n">
-        <v>179.8186336660424</v>
+        <v>179.8082515568856</v>
       </c>
       <c r="F82">
         <f>IF(AND(E82&gt;=C82,E82&lt;=D82), "PASS", "FAIL")</f>
@@ -1995,7 +1995,7 @@
         <v>60.25</v>
       </c>
       <c r="E83" t="n">
-        <v>60.26304637721221</v>
+        <v>60.24495290608287</v>
       </c>
       <c r="F83">
         <f>IF(AND(E83&gt;=C83,E83&lt;=D83), "PASS", "FAIL")</f>
@@ -2013,7 +2013,7 @@
         <v>120.25</v>
       </c>
       <c r="E84" t="n">
-        <v>120.2972119614733</v>
+        <v>120.2447823746622</v>
       </c>
       <c r="F84">
         <f>IF(AND(E84&gt;=C84,E84&lt;=D84), "PASS", "FAIL")</f>
@@ -2054,7 +2054,7 @@
         <v>60.25</v>
       </c>
       <c r="E86" t="n">
-        <v>60.23295852263566</v>
+        <v>60.20701054828241</v>
       </c>
       <c r="F86">
         <f>IF(AND(E86&gt;=C86,E86&lt;=D86), "PASS", "FAIL")</f>
@@ -2072,7 +2072,7 @@
         <v>120.25</v>
       </c>
       <c r="E87" t="n">
-        <v>120.2331134184667</v>
+        <v>120.167535693746</v>
       </c>
       <c r="F87">
         <f>IF(AND(E87&gt;=C87,E87&lt;=D87), "PASS", "FAIL")</f>
@@ -2113,7 +2113,7 @@
         <v>60.25</v>
       </c>
       <c r="E89" t="n">
-        <v>60.21943581112865</v>
+        <v>60.20570264038873</v>
       </c>
       <c r="F89">
         <f>IF(AND(E89&gt;=C89,E89&lt;=D89), "PASS", "FAIL")</f>
@@ -2131,7 +2131,7 @@
         <v>120.25</v>
       </c>
       <c r="E90" t="n">
-        <v>120.2084549933066</v>
+        <v>119.8126910889515</v>
       </c>
       <c r="F90">
         <f>IF(AND(E90&gt;=C90,E90&lt;=D90), "PASS", "FAIL")</f>

</xml_diff>